<commit_message>
measure_results working except for the win calculations
</commit_message>
<xml_diff>
--- a/predict/2023/saved/results.xlsx
+++ b/predict/2023/saved/results.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="10">
   <si>
     <t>Index</t>
   </si>
@@ -32,6 +32,18 @@
   </si>
   <si>
     <t>Percent Correct</t>
+  </si>
+  <si>
+    <t>01</t>
+  </si>
+  <si>
+    <t>03</t>
+  </si>
+  <si>
+    <t>02</t>
+  </si>
+  <si>
+    <t>100%</t>
   </si>
 </sst>
 </file>
@@ -389,7 +401,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -419,20 +431,60 @@
       <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2">
-        <v>1</v>
+      <c r="B2" t="s">
+        <v>6</v>
       </c>
       <c r="C2">
+        <v>94</v>
+      </c>
+      <c r="D2">
+        <v>37</v>
+      </c>
+      <c r="E2">
+        <v>57</v>
+      </c>
+      <c r="F2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3">
         <v>2</v>
       </c>
-      <c r="D2">
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3">
+        <v>75</v>
+      </c>
+      <c r="D3">
+        <v>24</v>
+      </c>
+      <c r="E3">
+        <v>51</v>
+      </c>
+      <c r="F3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4">
         <v>3</v>
       </c>
-      <c r="E2">
-        <v>4</v>
-      </c>
-      <c r="F2">
-        <v>5</v>
+      <c r="B4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4">
+        <v>85</v>
+      </c>
+      <c r="D4">
+        <v>30</v>
+      </c>
+      <c r="E4">
+        <v>55</v>
+      </c>
+      <c r="F4" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
all fixed ready to update master and tag the release
</commit_message>
<xml_diff>
--- a/predict/2023/saved/results.xlsx
+++ b/predict/2023/saved/results.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="37">
   <si>
     <t>Index</t>
   </si>
@@ -34,16 +34,97 @@
     <t>Percent Correct</t>
   </si>
   <si>
-    <t>01</t>
-  </si>
-  <si>
-    <t>03</t>
-  </si>
-  <si>
-    <t>02</t>
+    <t>013</t>
+  </si>
+  <si>
+    <t>015</t>
+  </si>
+  <si>
+    <t>bowls</t>
+  </si>
+  <si>
+    <t>004</t>
+  </si>
+  <si>
+    <t>001</t>
+  </si>
+  <si>
+    <t>011</t>
+  </si>
+  <si>
+    <t>007</t>
+  </si>
+  <si>
+    <t>014</t>
+  </si>
+  <si>
+    <t>006</t>
+  </si>
+  <si>
+    <t>003</t>
+  </si>
+  <si>
+    <t>009</t>
+  </si>
+  <si>
+    <t>002</t>
+  </si>
+  <si>
+    <t>005</t>
+  </si>
+  <si>
+    <t>008</t>
+  </si>
+  <si>
+    <t>012</t>
+  </si>
+  <si>
+    <t>010</t>
+  </si>
+  <si>
+    <t>totals</t>
+  </si>
+  <si>
+    <t>68%</t>
   </si>
   <si>
     <t>100%</t>
+  </si>
+  <si>
+    <t>81%</t>
+  </si>
+  <si>
+    <t>69%</t>
+  </si>
+  <si>
+    <t>61%</t>
+  </si>
+  <si>
+    <t>70%</t>
+  </si>
+  <si>
+    <t>57%</t>
+  </si>
+  <si>
+    <t>50%</t>
+  </si>
+  <si>
+    <t>67%</t>
+  </si>
+  <si>
+    <t>71%</t>
+  </si>
+  <si>
+    <t>78%</t>
+  </si>
+  <si>
+    <t>65%</t>
+  </si>
+  <si>
+    <t>66%</t>
+  </si>
+  <si>
+    <t>77%</t>
   </si>
 </sst>
 </file>
@@ -401,7 +482,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:F18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -435,16 +516,16 @@
         <v>6</v>
       </c>
       <c r="C2">
-        <v>94</v>
+        <v>65</v>
       </c>
       <c r="D2">
-        <v>37</v>
+        <v>5</v>
       </c>
       <c r="E2">
-        <v>57</v>
+        <v>41</v>
       </c>
       <c r="F2" t="s">
-        <v>9</v>
+        <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -455,16 +536,16 @@
         <v>7</v>
       </c>
       <c r="C3">
-        <v>75</v>
+        <v>1</v>
       </c>
       <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+      <c r="F3" t="s">
         <v>24</v>
-      </c>
-      <c r="E3">
-        <v>51</v>
-      </c>
-      <c r="F3" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -475,16 +556,296 @@
         <v>8</v>
       </c>
       <c r="C4">
+        <v>43</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4">
+        <v>34</v>
+      </c>
+      <c r="F4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5">
+        <v>67</v>
+      </c>
+      <c r="D5">
+        <v>5</v>
+      </c>
+      <c r="E5">
+        <v>43</v>
+      </c>
+      <c r="F5" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6">
+        <v>94</v>
+      </c>
+      <c r="D6">
+        <v>37</v>
+      </c>
+      <c r="E6">
+        <v>35</v>
+      </c>
+      <c r="F6" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7">
+        <v>65</v>
+      </c>
+      <c r="D7">
+        <v>2</v>
+      </c>
+      <c r="E7">
+        <v>44</v>
+      </c>
+      <c r="F7" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8">
+        <v>55</v>
+      </c>
+      <c r="D8">
+        <v>4</v>
+      </c>
+      <c r="E8">
+        <v>29</v>
+      </c>
+      <c r="F8" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C9">
+        <v>10</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+      <c r="E9">
+        <v>5</v>
+      </c>
+      <c r="F9" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>14</v>
+      </c>
+      <c r="C10">
+        <v>51</v>
+      </c>
+      <c r="D10">
+        <v>6</v>
+      </c>
+      <c r="E10">
+        <v>30</v>
+      </c>
+      <c r="F10" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>15</v>
+      </c>
+      <c r="C11">
+        <v>75</v>
+      </c>
+      <c r="D11">
+        <v>24</v>
+      </c>
+      <c r="E11">
+        <v>36</v>
+      </c>
+      <c r="F11" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>16</v>
+      </c>
+      <c r="C12">
+        <v>54</v>
+      </c>
+      <c r="D12">
+        <v>3</v>
+      </c>
+      <c r="E12">
+        <v>40</v>
+      </c>
+      <c r="F12" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>17</v>
+      </c>
+      <c r="C13">
         <v>85</v>
       </c>
-      <c r="D4">
+      <c r="D13">
         <v>30</v>
       </c>
-      <c r="E4">
-        <v>55</v>
-      </c>
-      <c r="F4" t="s">
-        <v>9</v>
+      <c r="E13">
+        <v>36</v>
+      </c>
+      <c r="F13" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>18</v>
+      </c>
+      <c r="C14">
+        <v>59</v>
+      </c>
+      <c r="D14">
+        <v>6</v>
+      </c>
+      <c r="E14">
+        <v>35</v>
+      </c>
+      <c r="F14" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
+        <v>19</v>
+      </c>
+      <c r="C15">
+        <v>54</v>
+      </c>
+      <c r="D15">
+        <v>1</v>
+      </c>
+      <c r="E15">
+        <v>35</v>
+      </c>
+      <c r="F15" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16" t="s">
+        <v>20</v>
+      </c>
+      <c r="C16">
+        <v>68</v>
+      </c>
+      <c r="D16">
+        <v>6</v>
+      </c>
+      <c r="E16">
+        <v>48</v>
+      </c>
+      <c r="F16" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17" t="s">
+        <v>21</v>
+      </c>
+      <c r="C17">
+        <v>65</v>
+      </c>
+      <c r="D17">
+        <v>7</v>
+      </c>
+      <c r="E17">
+        <v>33</v>
+      </c>
+      <c r="F17" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18" t="s">
+        <v>22</v>
+      </c>
+      <c r="C18">
+        <v>911</v>
+      </c>
+      <c r="D18">
+        <v>137</v>
+      </c>
+      <c r="E18">
+        <v>525</v>
+      </c>
+      <c r="F18" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>